<commit_message>
parentesi di alex mortacci tua
</commit_message>
<xml_diff>
--- a/DivisioneCompitiProgetto.xlsx
+++ b/DivisioneCompitiProgetto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niccolò\Documents\GitHub\WWFos_plus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07BA7844-C1C8-4856-9A84-A27AC93930CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D50680-82DC-40F4-A3DA-D64651BC6BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7665" yWindow="810" windowWidth="25440" windowHeight="18585" xr2:uid="{162DB40B-610E-44D7-B799-C2D70BE17169}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{162DB40B-610E-44D7-B799-C2D70BE17169}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>initPcbs</t>
   </si>
@@ -106,14 +106,25 @@
   </si>
   <si>
     <t>andre</t>
+  </si>
+  <si>
+    <t>fatta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -171,13 +182,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -495,7 +507,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,6 +525,9 @@
       <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -524,6 +539,9 @@
       <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -535,6 +553,9 @@
       <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -546,6 +567,9 @@
       <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -574,6 +598,9 @@
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="E6" s="5">
         <v>3</v>
       </c>
@@ -591,6 +618,9 @@
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="E7" s="3">
         <v>4</v>
       </c>
@@ -606,6 +636,7 @@
       <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -706,10 +737,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E00C5A350B8B864FA4BB6364DB87AFA5" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b03546160d7af3751660de6bf9eb727a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fe3a730e-302a-4df5-bd37-d9344ad5dd39" xmlns:ns4="59517204-b887-420f-893f-e0f09dd2c946" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a2fc8f87c45d55b23d30fe2f981dfbf9" ns3:_="" ns4:_="">
     <xsd:import namespace="fe3a730e-302a-4df5-bd37-d9344ad5dd39"/>
@@ -918,22 +965,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6ADF2E5-66BF-436E-A5DE-15F1AF697C78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fe3a730e-302a-4df5-bd37-d9344ad5dd39"/>
+    <ds:schemaRef ds:uri="59517204-b887-420f-893f-e0f09dd2c946"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6168705-F75C-4995-B7F0-B5C55A72CEAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A39DC78-4D5D-4213-A8CB-8E167CA8B9F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -950,29 +1007,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6168705-F75C-4995-B7F0-B5C55A72CEAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6ADF2E5-66BF-436E-A5DE-15F1AF697C78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fe3a730e-302a-4df5-bd37-d9344ad5dd39"/>
-    <ds:schemaRef ds:uri="59517204-b887-420f-893f-e0f09dd2c946"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fatta quinta funzione + bugfix codice
</commit_message>
<xml_diff>
--- a/DivisioneCompitiProgetto.xlsx
+++ b/DivisioneCompitiProgetto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niccolò\Documents\GitHub\WWFos_plus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D50680-82DC-40F4-A3DA-D64651BC6BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC097ECF-203D-4848-860C-A32670FD6266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{162DB40B-610E-44D7-B799-C2D70BE17169}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>initPcbs</t>
   </si>
@@ -182,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -190,6 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -507,7 +508,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,6 +582,9 @@
       <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="E5" s="4">
         <v>3</v>
       </c>
@@ -598,7 +602,7 @@
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="5">
@@ -742,18 +746,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -966,6 +970,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6168705-F75C-4995-B7F0-B5C55A72CEAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6ADF2E5-66BF-436E-A5DE-15F1AF697C78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -978,14 +990,6 @@
     <ds:schemaRef ds:uri="59517204-b887-420f-893f-e0f09dd2c946"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6168705-F75C-4995-B7F0-B5C55A72CEAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>